<commit_message>
removed test cases from testsuite collection
</commit_message>
<xml_diff>
--- a/ExcelFiles/file_example_XLSX_10.xlsx
+++ b/ExcelFiles/file_example_XLSX_10.xlsx
@@ -2,20 +2,20 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookPr backupFile="false" date1904="false" showObjects="all"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="205" firstSheet="0" activeTab="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="205" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" r:id="rId2" sheetId="1" state="visible"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr iterate="false" iterateCount="100" iterateDelta="0.001" refMode="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1482" uniqueCount="1435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1512" uniqueCount="1463">
   <si>
     <t>First Name</t>
   </si>
@@ -4320,6 +4320,90 @@
   </si>
   <si>
     <t>8608</t>
+  </si>
+  <si>
+    <t>416489317</t>
+  </si>
+  <si>
+    <t>8779</t>
+  </si>
+  <si>
+    <t>941930440</t>
+  </si>
+  <si>
+    <t>6618</t>
+  </si>
+  <si>
+    <t>201335124</t>
+  </si>
+  <si>
+    <t>8038</t>
+  </si>
+  <si>
+    <t>792132756</t>
+  </si>
+  <si>
+    <t>7022</t>
+  </si>
+  <si>
+    <t>428986907</t>
+  </si>
+  <si>
+    <t>1568</t>
+  </si>
+  <si>
+    <t>267788365</t>
+  </si>
+  <si>
+    <t>333545900</t>
+  </si>
+  <si>
+    <t>8475</t>
+  </si>
+  <si>
+    <t>900123606</t>
+  </si>
+  <si>
+    <t>9471</t>
+  </si>
+  <si>
+    <t>836455326</t>
+  </si>
+  <si>
+    <t>9116</t>
+  </si>
+  <si>
+    <t>805445054</t>
+  </si>
+  <si>
+    <t>1286</t>
+  </si>
+  <si>
+    <t>212848898</t>
+  </si>
+  <si>
+    <t>767236544</t>
+  </si>
+  <si>
+    <t>1863</t>
+  </si>
+  <si>
+    <t>783495863</t>
+  </si>
+  <si>
+    <t>7114</t>
+  </si>
+  <si>
+    <t>394541246</t>
+  </si>
+  <si>
+    <t>6758</t>
+  </si>
+  <si>
+    <t>435238503</t>
+  </si>
+  <si>
+    <t>4738</t>
   </si>
 </sst>
 </file>
@@ -4367,7 +4451,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border diagonalDown="false" diagonalUp="false">
       <left/>
       <right/>
       <top/>
@@ -4376,55 +4460,55 @@
     </border>
   </borders>
   <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
+    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
+    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
+    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
+    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
+    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -4434,10 +4518,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K18" activeCellId="0" sqref="K18"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="K18" activeCellId="0" pane="topLeft" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -4445,7 +4529,7 @@
     <col min="1" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1" s="1">
       <c r="A1" s="1" t="n">
         <v>0</v>
       </c>
@@ -4471,9 +4555,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
       <c r="A2" s="0" t="s">
-        <v>1406</v>
+        <v>1435</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>7</v>
@@ -4494,12 +4578,12 @@
         <v>11</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>1407</v>
+        <v>1436</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="3">
       <c r="A3" s="0" t="s">
-        <v>1408</v>
+        <v>1437</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>12</v>
@@ -4520,12 +4604,12 @@
         <v>15</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>1409</v>
+        <v>1438</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="4">
       <c r="A4" s="0" t="s">
-        <v>1410</v>
+        <v>1439</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>16</v>
@@ -4546,12 +4630,12 @@
         <v>20</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>1411</v>
+        <v>1440</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="5">
       <c r="A5" s="0" t="s">
-        <v>1412</v>
+        <v>1441</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>21</v>
@@ -4572,12 +4656,12 @@
         <v>11</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>1413</v>
+        <v>1442</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="6">
       <c r="A6" s="0" t="s">
-        <v>1414</v>
+        <v>1443</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>23</v>
@@ -4598,12 +4682,12 @@
         <v>15</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>1415</v>
+        <v>1444</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="7">
       <c r="A7" s="0" t="s">
-        <v>1416</v>
+        <v>1445</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>25</v>
@@ -4624,12 +4708,12 @@
         <v>20</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>1417</v>
+        <v>1064</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="8">
       <c r="A8" s="0" t="s">
-        <v>1418</v>
+        <v>1446</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>27</v>
@@ -4650,12 +4734,12 @@
         <v>11</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>1419</v>
+        <v>1447</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="9">
       <c r="A9" s="0" t="s">
-        <v>1420</v>
+        <v>1448</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>29</v>
@@ -4676,12 +4760,12 @@
         <v>15</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>1421</v>
+        <v>1449</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="10">
       <c r="A10" s="0" t="s">
-        <v>1422</v>
+        <v>1450</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>31</v>
@@ -4702,114 +4786,114 @@
         <v>20</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>1423</v>
+        <v>1451</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.65" outlineLevel="0" r="11">
       <c r="A11" t="s">
-        <v>1424</v>
+        <v>1452</v>
       </c>
       <c r="C11" t="s">
         <v>606</v>
       </c>
       <c r="H11" t="s">
-        <v>1425</v>
+        <v>1453</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.65" outlineLevel="0" r="12">
       <c r="A12" t="s">
-        <v>1426</v>
+        <v>1454</v>
       </c>
       <c r="C12" t="s">
         <v>215</v>
       </c>
       <c r="H12" t="s">
-        <v>1427</v>
+        <v>681</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.65" outlineLevel="0" r="13">
       <c r="A13" t="s">
-        <v>1428</v>
+        <v>1455</v>
       </c>
       <c r="C13" t="s">
         <v>609</v>
       </c>
       <c r="H13" t="s">
-        <v>1429</v>
+        <v>1456</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.65" outlineLevel="0" r="14">
       <c r="A14" t="s">
-        <v>1430</v>
+        <v>1457</v>
       </c>
       <c r="C14" t="s">
         <v>611</v>
       </c>
       <c r="H14" t="s">
-        <v>1249</v>
+        <v>1458</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.65" outlineLevel="0" r="15">
       <c r="A15" t="s">
-        <v>1431</v>
+        <v>1459</v>
       </c>
       <c r="C15" t="s">
         <v>613</v>
       </c>
       <c r="H15" t="s">
-        <v>1432</v>
+        <v>1460</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.65" outlineLevel="0" r="16">
       <c r="A16" t="s">
-        <v>1433</v>
+        <v>1461</v>
       </c>
       <c r="C16" t="s">
         <v>615</v>
       </c>
       <c r="H16" t="s">
-        <v>1434</v>
+        <v>1462</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="18" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="19" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="20" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="21" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="22" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="23" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="24" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="25" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="26" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="27" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="28" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="29" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="30" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="31" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="32" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="33" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="34" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="35" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="36" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="37" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="38" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="39" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="40" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="41" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="42" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="43" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="44" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="45" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="46" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="47" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="48" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="49" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="50" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="51" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.65" outlineLevel="0" r="17"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.65" outlineLevel="0" r="18"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.65" outlineLevel="0" r="19"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.65" outlineLevel="0" r="20"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.65" outlineLevel="0" r="21"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.65" outlineLevel="0" r="22"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.65" outlineLevel="0" r="23"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.65" outlineLevel="0" r="24"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.65" outlineLevel="0" r="25"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.65" outlineLevel="0" r="26"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.65" outlineLevel="0" r="27"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.65" outlineLevel="0" r="28"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.65" outlineLevel="0" r="29"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.65" outlineLevel="0" r="30"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.65" outlineLevel="0" r="31"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.65" outlineLevel="0" r="32"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.65" outlineLevel="0" r="33"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.65" outlineLevel="0" r="34"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.65" outlineLevel="0" r="35"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.65" outlineLevel="0" r="36"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.65" outlineLevel="0" r="37"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.65" outlineLevel="0" r="38"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.65" outlineLevel="0" r="39"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.65" outlineLevel="0" r="40"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.65" outlineLevel="0" r="41"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.65" outlineLevel="0" r="42"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.65" outlineLevel="0" r="43"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.65" outlineLevel="0" r="44"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.65" outlineLevel="0" r="45"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.65" outlineLevel="0" r="46"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.65" outlineLevel="0" r="47"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.65" outlineLevel="0" r="48"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.65" outlineLevel="0" r="49"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.65" outlineLevel="0" r="50"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.65" outlineLevel="0" r="51"/>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="true" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>